<commit_message>
updated data2 and plot
</commit_message>
<xml_diff>
--- a/upa_data2.xlsx
+++ b/upa_data2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterhiggins/Documents/RCode/upa_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358810EA-841D-D44E-9755-A6D953CC1800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DDC714-CC4C-D543-BC6E-110B6D661557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1400" yWindow="4400" windowWidth="16000" windowHeight="24840" xr2:uid="{ED0D8109-9F35-4F71-B5E9-D6058A382527}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="14">
   <si>
     <t>patient</t>
   </si>
@@ -428,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A804B8-38C6-443E-9FBD-3CF9D8FA977C}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -464,13 +464,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="1">
-        <v>44712.293749999997</v>
+        <v>44713.023611111108</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2">
-        <v>2.2999999999999998</v>
+        <v>1.7</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -487,13 +487,13 @@
         <v>7</v>
       </c>
       <c r="B3" s="1">
-        <v>44711.636111111111</v>
+        <v>44712.293749999997</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>24</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -513,10 +513,10 @@
         <v>44711.636111111111</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D4">
-        <v>3.4</v>
+        <v>24</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -533,13 +533,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>44711.107638888891</v>
+        <v>44711.636111111111</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
       <c r="D5">
-        <v>3.9</v>
+        <v>3.4</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -556,13 +556,13 @@
         <v>7</v>
       </c>
       <c r="B6" s="1">
-        <v>44710.276388888888</v>
+        <v>44711.107638888891</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6">
-        <v>5.5</v>
+        <v>3.9</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -579,13 +579,13 @@
         <v>7</v>
       </c>
       <c r="B7" s="1">
-        <v>44709.197222222225</v>
+        <v>44710.276388888888</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7">
-        <v>11.7</v>
+        <v>5.5</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -605,10 +605,10 @@
         <v>44709.197222222225</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <v>29</v>
+        <v>11.7</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -625,13 +625,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>44708.301388888889</v>
+        <v>44709.197222222225</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D9">
-        <v>23.4</v>
+        <v>29</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -648,16 +648,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="1">
-        <v>44707.381944444445</v>
+        <v>44708.301388888889</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>42</v>
+        <v>23.4</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="1">
         <v>44708.586111111108</v>
@@ -671,13 +671,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="1">
-        <v>44707.289583333331</v>
+        <v>44707.381944444445</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D11">
-        <v>14.5</v>
+        <v>42</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -691,22 +691,22 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1">
-        <v>44712.895833333336</v>
+        <v>44707.289583333331</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="D12">
-        <v>3.4</v>
+        <v>14.5</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="1">
-        <v>44710.472916666666</v>
+        <v>44708.586111111108</v>
       </c>
       <c r="G12" t="s">
         <v>6</v>
@@ -717,13 +717,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>44711.875694444447</v>
+        <v>44712.895833333336</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>3.4</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -740,13 +740,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="1">
-        <v>44710.945833333331</v>
+        <v>44711.875694444447</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -763,16 +763,16 @@
         <v>11</v>
       </c>
       <c r="B15" s="1">
-        <v>44710.372916666667</v>
+        <v>44710.945833333331</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
       </c>
       <c r="D15">
-        <v>13.4</v>
+        <v>10</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="1">
         <v>44710.472916666666</v>
@@ -786,13 +786,13 @@
         <v>11</v>
       </c>
       <c r="B16" s="1">
-        <v>44709.368055555555</v>
+        <v>44710.372916666667</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="D16">
-        <v>13.3</v>
+        <v>13.4</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -809,13 +809,13 @@
         <v>11</v>
       </c>
       <c r="B17" s="1">
-        <v>44708.811805555553</v>
+        <v>44709.368055555555</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D17">
-        <v>113</v>
+        <v>13.3</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -835,10 +835,10 @@
         <v>44708.811805555553</v>
       </c>
       <c r="C18" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D18">
-        <v>17.399999999999999</v>
+        <v>113</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -852,25 +852,25 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" s="1">
-        <v>44713.292361111111</v>
+        <v>44708.811805555553</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
       </c>
       <c r="D19">
-        <v>0.2</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" s="1">
-        <v>44708.879166666666</v>
+        <v>44710.472916666666</v>
       </c>
       <c r="G19" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
@@ -878,13 +878,13 @@
         <v>12</v>
       </c>
       <c r="B20" s="1">
-        <v>44711.861111111109</v>
+        <v>44713.292361111111</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="D20">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -901,13 +901,13 @@
         <v>12</v>
       </c>
       <c r="B21" s="1">
-        <v>44710.865277777775</v>
+        <v>44711.861111111109</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="D21">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -924,13 +924,13 @@
         <v>12</v>
       </c>
       <c r="B22" s="1">
-        <v>44709.899305555555</v>
+        <v>44710.865277777775</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
       </c>
       <c r="D22">
-        <v>2.4</v>
+        <v>0.9</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -947,13 +947,13 @@
         <v>12</v>
       </c>
       <c r="B23" s="1">
-        <v>44708.965277777781</v>
+        <v>44709.899305555555</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
       </c>
       <c r="D23">
-        <v>4.3</v>
+        <v>2.4</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -970,16 +970,16 @@
         <v>12</v>
       </c>
       <c r="B24" s="1">
-        <v>44706.989583333336</v>
+        <v>44708.965277777781</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
       </c>
       <c r="D24">
-        <v>2.8</v>
+        <v>4.3</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="1">
         <v>44708.879166666666</v>
@@ -988,9 +988,32 @@
         <v>13</v>
       </c>
     </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="1">
+        <v>44706.989583333336</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>2.8</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <v>44708.879166666666</v>
+      </c>
+      <c r="G25" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G11">
-    <sortCondition descending="1" ref="B2:B11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G12">
+    <sortCondition descending="1" ref="B3:B12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added new data June 2
</commit_message>
<xml_diff>
--- a/upa_data2.xlsx
+++ b/upa_data2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterhiggins/Documents/RCode/upa_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DDC714-CC4C-D543-BC6E-110B6D661557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63878681-D9FA-334A-9DC7-B13062178319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1400" yWindow="4400" windowWidth="16000" windowHeight="24840" xr2:uid="{ED0D8109-9F35-4F71-B5E9-D6058A382527}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="14">
   <si>
     <t>patient</t>
   </si>
@@ -428,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A804B8-38C6-443E-9FBD-3CF9D8FA977C}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -717,13 +717,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>44712.895833333336</v>
+        <v>44714.007638888892</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="D13">
-        <v>3.4</v>
+        <v>2.6</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -740,13 +740,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="1">
-        <v>44711.875694444447</v>
+        <v>44712.895833333336</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="D14">
-        <v>6</v>
+        <v>3.4</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -763,13 +763,13 @@
         <v>11</v>
       </c>
       <c r="B15" s="1">
-        <v>44710.945833333331</v>
+        <v>44711.875694444447</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
       </c>
       <c r="D15">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -786,16 +786,16 @@
         <v>11</v>
       </c>
       <c r="B16" s="1">
-        <v>44710.372916666667</v>
+        <v>44710.945833333331</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="D16">
-        <v>13.4</v>
+        <v>10</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="1">
         <v>44710.472916666666</v>
@@ -809,13 +809,13 @@
         <v>11</v>
       </c>
       <c r="B17" s="1">
-        <v>44709.368055555555</v>
+        <v>44710.372916666667</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="D17">
-        <v>13.3</v>
+        <v>13.4</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -832,13 +832,13 @@
         <v>11</v>
       </c>
       <c r="B18" s="1">
-        <v>44708.811805555553</v>
+        <v>44709.368055555555</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D18">
-        <v>113</v>
+        <v>13.3</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -858,10 +858,10 @@
         <v>44708.811805555553</v>
       </c>
       <c r="C19" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D19">
-        <v>17.399999999999999</v>
+        <v>113</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -875,25 +875,25 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" s="1">
-        <v>44713.292361111111</v>
+        <v>44708.811805555553</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="D20">
-        <v>0.2</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" s="1">
-        <v>44708.879166666666</v>
+        <v>44710.472916666666</v>
       </c>
       <c r="G20" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
@@ -901,13 +901,13 @@
         <v>12</v>
       </c>
       <c r="B21" s="1">
-        <v>44711.861111111109</v>
+        <v>44713.292361111111</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="D21">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -924,13 +924,13 @@
         <v>12</v>
       </c>
       <c r="B22" s="1">
-        <v>44710.865277777775</v>
+        <v>44711.861111111109</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
       </c>
       <c r="D22">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -947,13 +947,13 @@
         <v>12</v>
       </c>
       <c r="B23" s="1">
-        <v>44709.899305555555</v>
+        <v>44710.865277777775</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
       </c>
       <c r="D23">
-        <v>2.4</v>
+        <v>0.9</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -970,13 +970,13 @@
         <v>12</v>
       </c>
       <c r="B24" s="1">
-        <v>44708.965277777781</v>
+        <v>44709.899305555555</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
       </c>
       <c r="D24">
-        <v>4.3</v>
+        <v>2.4</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -993,21 +993,44 @@
         <v>12</v>
       </c>
       <c r="B25" s="1">
-        <v>44706.989583333336</v>
+        <v>44708.965277777781</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
       </c>
       <c r="D25">
-        <v>2.8</v>
+        <v>4.3</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="1">
         <v>44708.879166666666</v>
       </c>
       <c r="G25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="1">
+        <v>44706.989583333336</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>2.8</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>44708.879166666666</v>
+      </c>
+      <c r="G26" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated colors, anonymized patient id
</commit_message>
<xml_diff>
--- a/upa_data2.xlsx
+++ b/upa_data2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterhiggins/Documents/RCode/upa_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63878681-D9FA-334A-9DC7-B13062178319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17093E1C-D19E-1941-806C-17410B00FE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1400" yWindow="4400" windowWidth="16000" windowHeight="24840" xr2:uid="{ED0D8109-9F35-4F71-B5E9-D6058A382527}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="11">
   <si>
     <t>patient</t>
   </si>
@@ -58,9 +58,6 @@
     <t>uc</t>
   </si>
   <si>
-    <t>mwz</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
@@ -68,12 +65,6 @@
   </si>
   <si>
     <t>esr</t>
-  </si>
-  <si>
-    <t>mar</t>
-  </si>
-  <si>
-    <t>tgh</t>
   </si>
   <si>
     <t>cd</t>
@@ -428,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A804B8-38C6-443E-9FBD-3CF9D8FA977C}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -444,10 +435,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -460,64 +451,64 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>7</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" s="1">
+        <v>44714.336805555555</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>0.8</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>44708.586111111108</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
         <v>44713.023611111108</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2">
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
         <v>1.7</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1">
-        <v>44708.586111111108</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>44708.586111111108</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
         <v>44712.293749999997</v>
       </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3">
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1">
-        <v>44708.586111111108</v>
-      </c>
-      <c r="G3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1">
-        <v>44711.636111111111</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>24</v>
-      </c>
       <c r="E4">
         <v>1</v>
       </c>
@@ -529,87 +520,87 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>7</v>
+      <c r="A5">
+        <v>1</v>
       </c>
       <c r="B5" s="1">
         <v>44711.636111111111</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D5">
+        <v>24</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>44708.586111111108</v>
+      </c>
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44711.636111111111</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6">
         <v>3.4</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1">
-        <v>44708.586111111108</v>
-      </c>
-      <c r="G5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>44708.586111111108</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
         <v>44711.107638888891</v>
       </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6">
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7">
         <v>3.9</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1">
-        <v>44708.586111111108</v>
-      </c>
-      <c r="G6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>44708.586111111108</v>
+      </c>
+      <c r="G7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
         <v>44710.276388888888</v>
       </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7">
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8">
         <v>5.5</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1">
-        <v>44708.586111111108</v>
-      </c>
-      <c r="G7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>44709.197222222225</v>
-      </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>11.7</v>
-      </c>
       <c r="E8">
         <v>1</v>
       </c>
@@ -621,86 +612,86 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>7</v>
+      <c r="A9">
+        <v>1</v>
       </c>
       <c r="B9" s="1">
         <v>44709.197222222225</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D9">
+        <v>11.7</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>44708.586111111108</v>
+      </c>
+      <c r="G9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44709.197222222225</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10">
         <v>29</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1">
-        <v>44708.586111111108</v>
-      </c>
-      <c r="G9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="1">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>44708.586111111108</v>
+      </c>
+      <c r="G10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
         <v>44708.301388888889</v>
       </c>
-      <c r="C10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10">
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11">
         <v>23.4</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1">
-        <v>44708.586111111108</v>
-      </c>
-      <c r="G10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="1">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>44708.586111111108</v>
+      </c>
+      <c r="G11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
         <v>44707.381944444445</v>
       </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11">
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12">
         <v>42</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
-        <v>44708.586111111108</v>
-      </c>
-      <c r="G11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="1">
-        <v>44707.289583333331</v>
-      </c>
-      <c r="C12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>14.5</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -713,40 +704,40 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
-        <v>11</v>
+      <c r="A13">
+        <v>1</v>
       </c>
       <c r="B13" s="1">
+        <v>44707.289583333331</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>14.5</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>44708.586111111108</v>
+      </c>
+      <c r="G13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1">
         <v>44714.007638888892</v>
       </c>
-      <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13">
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14">
         <v>2.6</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1">
-        <v>44710.472916666666</v>
-      </c>
-      <c r="G13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="1">
-        <v>44712.895833333336</v>
-      </c>
-      <c r="C14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>3.4</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -759,17 +750,17 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" t="s">
-        <v>11</v>
+      <c r="A15">
+        <v>2</v>
       </c>
       <c r="B15" s="1">
-        <v>44711.875694444447</v>
+        <v>44712.895833333336</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
       </c>
       <c r="D15">
-        <v>6</v>
+        <v>3.4</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -782,17 +773,17 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
-        <v>11</v>
+      <c r="A16">
+        <v>2</v>
       </c>
       <c r="B16" s="1">
-        <v>44710.945833333331</v>
+        <v>44711.875694444447</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="D16">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -805,20 +796,20 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
-        <v>11</v>
+      <c r="A17">
+        <v>2</v>
       </c>
       <c r="B17" s="1">
-        <v>44710.372916666667</v>
+        <v>44710.945833333331</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="D17">
-        <v>13.4</v>
+        <v>10</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="1">
         <v>44710.472916666666</v>
@@ -828,17 +819,17 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
-        <v>11</v>
+      <c r="A18">
+        <v>2</v>
       </c>
       <c r="B18" s="1">
-        <v>44709.368055555555</v>
+        <v>44710.372916666667</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
       </c>
       <c r="D18">
-        <v>13.3</v>
+        <v>13.4</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -851,17 +842,17 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
-        <v>11</v>
+      <c r="A19">
+        <v>2</v>
       </c>
       <c r="B19" s="1">
-        <v>44708.811805555553</v>
+        <v>44709.368055555555</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D19">
-        <v>113</v>
+        <v>13.3</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -874,17 +865,17 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A20" t="s">
-        <v>11</v>
+      <c r="A20">
+        <v>2</v>
       </c>
       <c r="B20" s="1">
         <v>44708.811805555553</v>
       </c>
       <c r="C20" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D20">
-        <v>17.399999999999999</v>
+        <v>113</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -897,40 +888,40 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
-        <v>12</v>
+      <c r="A21">
+        <v>2</v>
       </c>
       <c r="B21" s="1">
+        <v>44708.811805555553</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>44710.472916666666</v>
+      </c>
+      <c r="G21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" s="1">
         <v>44713.292361111111</v>
       </c>
-      <c r="C21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21">
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22">
         <v>0.2</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21" s="1">
-        <v>44708.879166666666</v>
-      </c>
-      <c r="G21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="1">
-        <v>44711.861111111109</v>
-      </c>
-      <c r="C22" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22">
-        <v>0.4</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -939,21 +930,21 @@
         <v>44708.879166666666</v>
       </c>
       <c r="G22" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
-        <v>12</v>
+      <c r="A23">
+        <v>3</v>
       </c>
       <c r="B23" s="1">
-        <v>44710.865277777775</v>
+        <v>44711.861111111109</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
       </c>
       <c r="D23">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -962,21 +953,21 @@
         <v>44708.879166666666</v>
       </c>
       <c r="G23" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A24" t="s">
-        <v>12</v>
+      <c r="A24">
+        <v>3</v>
       </c>
       <c r="B24" s="1">
-        <v>44709.899305555555</v>
+        <v>44710.865277777775</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
       </c>
       <c r="D24">
-        <v>2.4</v>
+        <v>0.9</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -985,21 +976,21 @@
         <v>44708.879166666666</v>
       </c>
       <c r="G24" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
-        <v>12</v>
+      <c r="A25">
+        <v>3</v>
       </c>
       <c r="B25" s="1">
-        <v>44708.965277777781</v>
+        <v>44709.899305555555</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
       </c>
       <c r="D25">
-        <v>4.3</v>
+        <v>2.4</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1008,35 +999,58 @@
         <v>44708.879166666666</v>
       </c>
       <c r="G25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A26" t="s">
-        <v>12</v>
+      <c r="A26">
+        <v>3</v>
       </c>
       <c r="B26" s="1">
-        <v>44706.989583333336</v>
+        <v>44708.965277777781</v>
       </c>
       <c r="C26" t="s">
         <v>2</v>
       </c>
       <c r="D26">
-        <v>2.8</v>
+        <v>4.3</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="1">
         <v>44708.879166666666</v>
       </c>
       <c r="G26" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27" s="1">
+        <v>44706.989583333336</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>2.8</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>44708.879166666666</v>
+      </c>
+      <c r="G27" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G12">
-    <sortCondition descending="1" ref="B3:B12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:G13">
+    <sortCondition descending="1" ref="B4:B13"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated upa data2, analysis. Plan to add patients 4-6
</commit_message>
<xml_diff>
--- a/upa_data2.xlsx
+++ b/upa_data2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterhiggins/Documents/RCode/upa_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17093E1C-D19E-1941-806C-17410B00FE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9298D4D-0609-6F4D-9469-E03BFD60587A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1400" yWindow="4400" windowWidth="16000" windowHeight="24840" xr2:uid="{ED0D8109-9F35-4F71-B5E9-D6058A382527}"/>
   </bookViews>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A804B8-38C6-443E-9FBD-3CF9D8FA977C}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1046,6 +1046,11 @@
       </c>
       <c r="G27" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>